<commit_message>
male→female header in BOM
</commit_message>
<xml_diff>
--- a/shield_driver_v0p3/production_v0/BOM.xlsx
+++ b/shield_driver_v0p3/production_v0/BOM.xlsx
@@ -49,10 +49,10 @@
     <t xml:space="preserve">P0-P3</t>
   </si>
   <si>
-    <t xml:space="preserve">2x2 male header, 0.1” pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">952-2119-ND</t>
+    <t xml:space="preserve">4 Position Receptacle Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A26452-ND</t>
   </si>
   <si>
     <t xml:space="preserve">Digikey</t>
@@ -115,6 +115,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,6 +137,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,44 +182,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,48 +240,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="22.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="35.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="22.16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -289,21 +295,21 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="J2" s="0" t="n">
+      <c r="H2" s="2" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="J2" s="2" t="n">
         <f aca="false">H2*B2</f>
-        <v>0.96</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,19 +322,19 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="7" t="n">
         <v>854</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="2" t="n">
         <v>0.97</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="2" t="n">
         <f aca="false">H3*B3</f>
         <v>0.97</v>
       </c>
@@ -343,19 +349,19 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="7" t="n">
         <v>137673</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="2" t="n">
         <v>0.45</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="2" t="n">
         <f aca="false">H4*B4</f>
         <v>0.45</v>
       </c>
@@ -370,19 +376,19 @@
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="2" t="n">
         <v>0.76</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="2" t="n">
         <f aca="false">H5*B5</f>
         <v>0.76</v>
       </c>
@@ -397,70 +403,70 @@
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="2" t="n">
         <v>0.74</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="2" t="n">
         <f aca="false">H6*B6</f>
         <v>0.74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="8" t="n">
+      <c r="A12" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="9" t="n">
+      <c r="E12" s="10" t="n">
         <v>855</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="2" t="n">
         <v>0.97</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="2" t="n">
         <f aca="false">H12*B12</f>
         <v>1.94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="2" t="n">
         <f aca="false">SUM(J2:J12)</f>
-        <v>5.82</v>
+        <v>11.7</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>